<commit_message>
Added VatRateCalculator with UT. Implemented VatCalculationController
</commit_message>
<xml_diff>
--- a/TaxRates/Data/Source/TaxRatesSource.xlsx
+++ b/TaxRates/Data/Source/TaxRatesSource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konrad\source\repos\TaxRates\TaxRates\Data\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0076F2D6-9A9D-4822-9F6E-FD8B2C86B9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D4141A-180D-4700-BA22-E672544070D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2475" windowWidth="21840" windowHeight="13290" xr2:uid="{395119C2-D707-4AC2-A850-F74D2427D2CA}"/>
   </bookViews>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAC7449-1696-4DE1-B104-F2771D916B47}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>